<commit_message>
this is change in dev branch
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Desktop\gitprctice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ashwini\git demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E4355-18CF-497E-AFB8-4301950B340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E95BC00-FDD7-4EA4-BB03-8DE5556A02B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12228" yWindow="540" windowWidth="10812" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">sr no </t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>des</t>
+  </si>
+  <si>
+    <t>pqr</t>
+  </si>
+  <si>
+    <t>pune</t>
   </si>
 </sst>
 </file>
@@ -363,15 +369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +387,11 @@
       <c r="C1">
         <v>2</v>
       </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -392,8 +401,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -402,6 +414,9 @@
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>